<commit_message>
refactoring: defining and disjoining booleanconditions from conditional expressions
</commit_message>
<xml_diff>
--- a/src/main/java/net/clementlevallois/umigon/heuristics/resources/en/en.xlsx
+++ b/src/main/java/net/clementlevallois/umigon/heuristics/resources/en/en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levallois\Google Drive\open\UmigonLambda\umigon-heuristics\src\main\java\net\clementlevallois\umigon\heuristics\resources\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFC009A-042E-4391-9FDA-AB490CB29D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B049A735-6C87-46B8-9726-80CE35EEAF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="871" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="871" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rules" sheetId="8" r:id="rId1"/>
@@ -23946,7 +23946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A550E3-CE74-4DC4-8CE4-1371722C8225}">
   <dimension ref="A1:C376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -26600,9 +26600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="16" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B84" sqref="B84:C84"/>
+      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>